<commit_message>
hlr and test case
hlr and test case for website saucedemo.com
</commit_message>
<xml_diff>
--- a/HLR and Testcase/hlr for loked out user.xlsx
+++ b/HLR and Testcase/hlr for loked out user.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ATRI ENTERPRISE\Documents\GitHub\Nirav_Tops\Assignment\HLR excel sheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ATRI ENTERPRISE\Documents\GitHub\Nirav_Tops\HLR and Testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB67F7B-81EA-4FDF-A32F-13B7808B0F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48520799-C6B8-407E-BBD8-72AB0714A1A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="56">
   <si>
     <t>functionality id</t>
   </si>
@@ -113,6 +113,100 @@
   </si>
   <si>
     <t>as per the expected result while getting click on login button show the display message properly but user has been locked out</t>
+  </si>
+  <si>
+    <t>check login button with blank username and blank password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user name: 
+password: </t>
+  </si>
+  <si>
+    <t>it is not showing the proper validation message</t>
+  </si>
+  <si>
+    <t>check login button with correct username and blank password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user name: locked_out_user
+password: </t>
+  </si>
+  <si>
+    <t>check login button with blank username and correct password</t>
+  </si>
+  <si>
+    <t>user name: 
+password: secret_sauce</t>
+  </si>
+  <si>
+    <t>check login button with username having special characters and correct password</t>
+  </si>
+  <si>
+    <t>user name: locked_out_user@@
+password: secret_sauce</t>
+  </si>
+  <si>
+    <t>check login button with correct username and having special characters with password</t>
+  </si>
+  <si>
+    <t>user name: locked_out_user
+password: secret_sauce@@</t>
+  </si>
+  <si>
+    <t>check login button with username having special characters and password as blank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user name: locked_out_user@@
+password: </t>
+  </si>
+  <si>
+    <t>check login button with blank username and having special characters with password</t>
+  </si>
+  <si>
+    <t>user name: 
+password: secret_sauce@@</t>
+  </si>
+  <si>
+    <t>check login button with username having digit and correct password</t>
+  </si>
+  <si>
+    <t>user name: locked_out_user123
+password: secret_sauce</t>
+  </si>
+  <si>
+    <t>check login button with correct user name and having digit with password</t>
+  </si>
+  <si>
+    <t>user name: locked_out_user
+password: secret_sauce123</t>
+  </si>
+  <si>
+    <t>check login button with username having white space between them and correct password</t>
+  </si>
+  <si>
+    <t>user name: locked out user  
+password: secret_sauce</t>
+  </si>
+  <si>
+    <t>check login button with correct username and white space between them in password</t>
+  </si>
+  <si>
+    <t>user name: locked_out_user
+password: secret sauce</t>
+  </si>
+  <si>
+    <t>check login button with username having white space between them and password as blank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user name: locked out user
+password: </t>
+  </si>
+  <si>
+    <t>check login button with username as blank and white space between them in password</t>
+  </si>
+  <si>
+    <t>user name: 
+password: secret sauce</t>
   </si>
 </sst>
 </file>
@@ -198,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -235,6 +329,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -630,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,148 +828,382 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-    </row>
-    <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-    </row>
-    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-    </row>
-    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-    </row>
-    <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-    </row>
-    <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-    </row>
-    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-    </row>
-    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-    </row>
-    <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-    </row>
-    <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-    </row>
-    <row r="15" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-    </row>
-    <row r="16" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
+    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13">
+        <v>2</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>4</v>
+      </c>
+      <c r="B5" s="13">
+        <v>2</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13">
+        <v>2</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>6</v>
+      </c>
+      <c r="B7" s="13">
+        <v>2</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="7" customFormat="1" ht="93.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>7</v>
+      </c>
+      <c r="B8" s="13">
+        <v>2</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
+        <v>8</v>
+      </c>
+      <c r="B9" s="13">
+        <v>2</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="7" customFormat="1" ht="93.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>9</v>
+      </c>
+      <c r="B10" s="13">
+        <v>2</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
+        <v>10</v>
+      </c>
+      <c r="B11" s="13">
+        <v>2</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
+        <v>11</v>
+      </c>
+      <c r="B12" s="13">
+        <v>2</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="13">
+        <v>2</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
+        <v>13</v>
+      </c>
+      <c r="B14" s="13">
+        <v>2</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="13">
+        <v>14</v>
+      </c>
+      <c r="B15" s="13">
+        <v>2</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
+        <v>15</v>
+      </c>
+      <c r="B16" s="13">
+        <v>2</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="12"/>

</xml_diff>